<commit_message>
Cleaned up the mobile design
</commit_message>
<xml_diff>
--- a/Shop_Reports.xlsx
+++ b/Shop_Reports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Month</t>
   </si>
@@ -34,28 +34,13 @@
     <t>Total Profit</t>
   </si>
   <si>
-    <t>February</t>
+    <t>July</t>
   </si>
   <si>
     <t>Shop 1</t>
   </si>
   <si>
     <t>Shop 2</t>
-  </si>
-  <si>
-    <t>Nzerekore</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>July</t>
   </si>
   <si>
     <t>Total Profit for all shops</t>
@@ -402,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,7 +426,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>290900</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -450,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>290900</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -461,293 +446,33 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>164800</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>39800</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>390900</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>390900</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>490900</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>490900</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>590900</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>590900</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>2178200</v>
-      </c>
-      <c r="D14">
-        <v>1835000</v>
-      </c>
-      <c r="E14">
-        <v>31800</v>
-      </c>
-      <c r="F14">
-        <v>343200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>3777400</v>
-      </c>
-      <c r="D15">
-        <v>3110000</v>
-      </c>
-      <c r="E15">
-        <v>37600</v>
-      </c>
-      <c r="F15">
-        <v>667400</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>620000</v>
-      </c>
-      <c r="D16">
-        <v>482000</v>
-      </c>
-      <c r="E16">
-        <v>3000</v>
-      </c>
-      <c r="F16">
-        <v>138000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2">
-        <v>1148600</v>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>39800</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added borrower registration and account updates
</commit_message>
<xml_diff>
--- a/Shop_Reports.xlsx
+++ b/Shop_Reports.xlsx
@@ -426,16 +426,16 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -446,16 +446,16 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>164800</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>125000</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>39800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -467,7 +467,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2">
-        <v>39800</v>
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting dollar conversions in account transfers
</commit_message>
<xml_diff>
--- a/Shop_Reports.xlsx
+++ b/Shop_Reports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>Month</t>
   </si>
@@ -34,13 +34,22 @@
     <t>Total Profit</t>
   </si>
   <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>Shop 2</t>
+  </si>
+  <si>
+    <t>Shop 1</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
     <t>August</t>
-  </si>
-  <si>
-    <t>Shop 2</t>
-  </si>
-  <si>
-    <t>Shop 1</t>
   </si>
   <si>
     <t>September</t>
@@ -396,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,16 +444,16 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>2403955</v>
+        <v>240000</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>168399.4</v>
       </c>
       <c r="E2">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>2403955</v>
+        <v>71600.60000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -475,16 +484,16 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>378370</v>
+        <v>240000</v>
       </c>
       <c r="D4">
-        <v>494.286</v>
+        <v>5980.1</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>377875.714</v>
+        <v>234019.9</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -515,16 +524,16 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>5600</v>
+        <v>239000</v>
       </c>
       <c r="D6">
-        <v>11960.2</v>
+        <v>168399.4</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F6">
-        <v>-6360.200000000001</v>
+        <v>70600.60000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -535,16 +544,16 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -555,16 +564,16 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>1660</v>
+        <v>2403955</v>
       </c>
       <c r="D8">
-        <v>2990.05</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>256</v>
       </c>
       <c r="F8">
-        <v>-1330.05</v>
+        <v>2403955</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -588,20 +597,140 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2">
-        <v>-1330.05</v>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>378370</v>
+      </c>
+      <c r="D10">
+        <v>494.286</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>377875.714</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>5600</v>
+      </c>
+      <c r="D12">
+        <v>11960.2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>-6360.200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>450</v>
+      </c>
+      <c r="D13">
+        <v>360</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>2452470</v>
+      </c>
+      <c r="D14">
+        <v>1797870.186</v>
+      </c>
+      <c r="E14">
+        <v>1290</v>
+      </c>
+      <c r="F14">
+        <v>654599.814</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <v>654599.814</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>